<commit_message>
Actualizar archivos de resultados (JSON y Excel) tras nueva ejecución del notebook
</commit_message>
<xml_diff>
--- a/Proyecto_Ofertas_Empleo/ofertas_procesadas.xlsx
+++ b/Proyecto_Ofertas_Empleo/ofertas_procesadas.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U47"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,30 +515,10 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>codigo_cuoc</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>ocupacion_cuoc</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>similitud</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>grupo_cuoc</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>fecha</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>salario_valor</t>
         </is>
@@ -604,18 +588,10 @@
           <t>Calle 59 13-33, Chapinero Edificio Pasaje Galvis, Oficina 124, segundo piso Te esperamos con tu hoja</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -661,18 +637,10 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+      <c r="P3" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -720,18 +688,10 @@
         </is>
       </c>
       <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="P4" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -791,24 +751,10 @@
           <t>Unilago (Cra. 15 78-33) Regístrate:</t>
         </is>
       </c>
-      <c r="P5" t="n">
-        <v>33551.008</v>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Inspector detective</t>
-        </is>
-      </c>
-      <c r="R5" t="n">
-        <v>67</v>
-      </c>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr"/>
+      <c r="P5" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -879,18 +825,10 @@
           <t>Metrópolis - Av. Carrera 68 75A - 50, Barrios Unidos. Confirma tu asistencia aquí:</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -926,18 +864,10 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1005,18 +935,10 @@
           <t>Calle 59 13-33, Chapinero Edificio Pasaje Galvis, Oficina 124, segundo piso Te esperamos con tu hoja</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr"/>
+      <c r="P8" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1064,18 +986,10 @@
         </is>
       </c>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="P9" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1135,24 +1049,10 @@
           <t>Unilago (Cra. 15 78-33) Regístrate:</t>
         </is>
       </c>
-      <c r="P10" t="n">
-        <v>33551.008</v>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Inspector detective</t>
-        </is>
-      </c>
-      <c r="R10" t="n">
-        <v>67</v>
-      </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr"/>
+      <c r="P10" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1223,18 +1123,10 @@
           <t>Metrópolis - Av. Carrera 68 75A - 50, Barrios Unidos. Confirma tu asistencia aquí :</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr"/>
+      <c r="P11" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1279,18 +1171,10 @@
         </is>
       </c>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="P12" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1359,18 +1243,10 @@
           <t>Fiesta Suba Cl. 147 101-56 Confirma tu asistencia aquí:</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr"/>
+      <c r="P13" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1434,18 +1310,10 @@
           <t>Plazoleta, entrada N 1 Centro Comercial Plaza Imperial (Av. Carrera 104 148-07).</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr"/>
+      <c r="P14" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1486,18 +1354,10 @@
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+      <c r="P15" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="n">
-        <v>0</v>
-      </c>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1551,18 +1411,10 @@
           <t>Plaza Imperial Conoce todos los detalles aquí:</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr"/>
+      <c r="P16" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1625,18 +1477,10 @@
           <t>Plaza Imperial Entrada 1 Del 30 de septiembre al 4 de octubre Lunes a viernes: 8 a.m. 4 p.m. Sábado:</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr"/>
+      <c r="P17" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="n">
-        <v>0</v>
-      </c>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1713,18 +1557,10 @@
           <t>Plaza Imperial, entrada 1 (Av. Carrera 104 148-07, entrada del Jumbo, junto al Éxito y la Av. Ciudad</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr"/>
+      <c r="P18" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1788,18 +1624,10 @@
           <t>Plazoleta, entrada N 1 Centro Comercial Plaza Imperial (Av. Carrera 104 148-07).</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr"/>
+      <c r="P19" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="n">
-        <v>0</v>
-      </c>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1844,18 +1672,10 @@
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
+      <c r="P20" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="n">
-        <v>0</v>
-      </c>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1906,18 +1726,10 @@
         </is>
       </c>
       <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
+      <c r="P21" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="n">
-        <v>0</v>
-      </c>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1970,18 +1782,10 @@
         </is>
       </c>
       <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="n">
-        <v>0</v>
-      </c>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2043,24 +1847,10 @@
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
-      <c r="P23" t="n">
-        <v>341</v>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>Técnicos y profesionales del nivel medio de servicios jurídicos, sociales y religiosos</t>
-        </is>
-      </c>
-      <c r="R23" t="n">
-        <v>60</v>
-      </c>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U23" t="n">
+      <c r="P23" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q23" t="n">
         <v>8000000</v>
       </c>
     </row>
@@ -2124,18 +1914,10 @@
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="n">
-        <v>0</v>
-      </c>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U24" t="n">
+      <c r="P24" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q24" t="n">
         <v>2109440</v>
       </c>
     </row>
@@ -2195,24 +1977,10 @@
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="n">
-        <v>32</v>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>TÉCNICOS Y PROFESIONALES DEL NIVEL MEDIO DE LA SALUD</t>
-        </is>
-      </c>
-      <c r="R25" t="n">
-        <v>70</v>
-      </c>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U25" t="n">
+      <c r="P25" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q25" t="n">
         <v>3906000</v>
       </c>
     </row>
@@ -2275,24 +2043,10 @@
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
-      <c r="P26" t="n">
-        <v>32112</v>
-      </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>Técnicos y tecnólogos en radioterapia</t>
-        </is>
-      </c>
-      <c r="R26" t="n">
-        <v>67</v>
-      </c>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U26" t="n">
+      <c r="P26" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q26" t="n">
         <v>2972000</v>
       </c>
     </row>
@@ -2356,24 +2110,10 @@
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="n">
-        <v>341</v>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>Técnicos y profesionales del nivel medio de servicios jurídicos, sociales y religiosos</t>
-        </is>
-      </c>
-      <c r="R27" t="n">
-        <v>60</v>
-      </c>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U27" t="n">
+      <c r="P27" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q27" t="n">
         <v>8000000</v>
       </c>
     </row>
@@ -2437,18 +2177,10 @@
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="n">
-        <v>0</v>
-      </c>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U28" t="n">
+      <c r="P28" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q28" t="n">
         <v>2109440</v>
       </c>
     </row>
@@ -2508,24 +2240,10 @@
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="n">
-        <v>32</v>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>TÉCNICOS Y PROFESIONALES DEL NIVEL MEDIO DE LA SALUD</t>
-        </is>
-      </c>
-      <c r="R29" t="n">
-        <v>70</v>
-      </c>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U29" t="n">
+      <c r="P29" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q29" t="n">
         <v>3906000</v>
       </c>
     </row>
@@ -2588,24 +2306,10 @@
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
-      <c r="P30" t="n">
-        <v>32112</v>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>Técnicos y tecnólogos en radioterapia</t>
-        </is>
-      </c>
-      <c r="R30" t="n">
-        <v>67</v>
-      </c>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U30" t="n">
+      <c r="P30" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q30" t="n">
         <v>2972000</v>
       </c>
     </row>
@@ -2686,18 +2390,10 @@
           <t>99 Nº18-02, Formulario:</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr"/>
+      <c r="P31" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="n">
-        <v>0</v>
-      </c>
-      <c r="S31" t="inlineStr"/>
-      <c r="T31" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2765,24 +2461,10 @@
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="n">
-        <v>42220.004</v>
-      </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>Asesor call center</t>
-        </is>
-      </c>
-      <c r="R32" t="n">
-        <v>100</v>
-      </c>
-      <c r="S32" t="inlineStr"/>
-      <c r="T32" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U32" t="inlineStr"/>
+      <c r="P32" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2857,18 +2539,10 @@
           <t>81b con Av Boyacá (Edificio Connecta) Regístrate aquí</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="n">
-        <v>0</v>
-      </c>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2908,18 +2582,10 @@
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="P34" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="n">
-        <v>0</v>
-      </c>
-      <c r="S34" t="inlineStr"/>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2956,18 +2622,10 @@
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
+      <c r="P35" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="n">
-        <v>0</v>
-      </c>
-      <c r="S35" t="inlineStr"/>
-      <c r="T35" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -3016,18 +2674,10 @@
       </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
+      <c r="P36" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="n">
-        <v>0</v>
-      </c>
-      <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -3064,18 +2714,10 @@
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
+      <c r="P37" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="n">
-        <v>0</v>
-      </c>
-      <c r="S37" t="inlineStr"/>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -3153,24 +2795,10 @@
           <t>75 69h 05, barrio Las Ferias CAMI Recuerda llevar tu hoja de vida y documento de identificación.</t>
         </is>
       </c>
-      <c r="P38" t="n">
-        <v>26531.002</v>
-      </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>Bailarín profesional</t>
-        </is>
-      </c>
-      <c r="R38" t="n">
-        <v>72</v>
-      </c>
-      <c r="S38" t="inlineStr"/>
-      <c r="T38" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U38" t="n">
+      <c r="P38" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q38" t="n">
         <v>1975692</v>
       </c>
     </row>
@@ -3215,18 +2843,10 @@
         </is>
       </c>
       <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
+      <c r="P39" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="n">
-        <v>0</v>
-      </c>
-      <c r="S39" t="inlineStr"/>
-      <c r="T39" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -3281,18 +2901,10 @@
           <t>Unilago (Cra. 15 78-33)</t>
         </is>
       </c>
-      <c r="P40" t="inlineStr"/>
+      <c r="P40" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="n">
-        <v>0</v>
-      </c>
-      <c r="S40" t="inlineStr"/>
-      <c r="T40" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3340,18 +2952,10 @@
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr"/>
+      <c r="P41" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="n">
-        <v>0</v>
-      </c>
-      <c r="S41" t="inlineStr"/>
-      <c r="T41" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3399,24 +3003,10 @@
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr"/>
-      <c r="P42" t="n">
-        <v>35121.038</v>
-      </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>Técnico de soporte en tecnología de la información</t>
-        </is>
-      </c>
-      <c r="R42" t="n">
-        <v>64</v>
-      </c>
-      <c r="S42" t="inlineStr"/>
-      <c r="T42" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U42" t="inlineStr"/>
+      <c r="P42" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3494,24 +3084,10 @@
           <t>75 69h 05, barrio Las Ferias CAMI Recuerda llevar tu hoja de vida y documento de identificación.</t>
         </is>
       </c>
-      <c r="P43" t="n">
-        <v>26531.002</v>
-      </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>Bailarín profesional</t>
-        </is>
-      </c>
-      <c r="R43" t="n">
-        <v>72</v>
-      </c>
-      <c r="S43" t="inlineStr"/>
-      <c r="T43" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U43" t="n">
+      <c r="P43" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="Q43" t="n">
         <v>1975692</v>
       </c>
     </row>
@@ -3578,18 +3154,10 @@
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
+      <c r="P44" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="n">
-        <v>0</v>
-      </c>
-      <c r="S44" t="inlineStr"/>
-      <c r="T44" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3636,18 +3204,10 @@
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr"/>
+      <c r="P45" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="n">
-        <v>0</v>
-      </c>
-      <c r="S45" t="inlineStr"/>
-      <c r="T45" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3683,18 +3243,10 @@
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
+      <c r="P46" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="n">
-        <v>0</v>
-      </c>
-      <c r="S46" t="inlineStr"/>
-      <c r="T46" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3759,18 +3311,10 @@
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
+      <c r="P47" s="2" t="n">
+        <v>45944</v>
+      </c>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="n">
-        <v>0</v>
-      </c>
-      <c r="S47" t="inlineStr"/>
-      <c r="T47" t="inlineStr">
-        <is>
-          <t>2025-10-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="U47" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>